<commit_message>
Create combined data file
Includes a couple of fixes discovered by insepcting the output data:
* convert datetimes to dates (the source data are all dates)
* correct the name of the source notes column
</commit_message>
<xml_diff>
--- a/tests/test_gp_data.xlsx
+++ b/tests/test_gp_data.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="71">
   <si>
     <t xml:space="preserve">Elector Number Prefix</t>
   </si>
@@ -89,6 +89,9 @@
   </si>
   <si>
     <t xml:space="preserve">1-5</t>
+  </si>
+  <si>
+    <t xml:space="preserve">   </t>
   </si>
   <si>
     <t xml:space="preserve">Date Last Knocked</t>
@@ -508,13 +511,13 @@
   </sheetPr>
   <dimension ref="A1:Y8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F18" activeCellId="0" sqref="F18"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="N1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="W14" activeCellId="0" sqref="W14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.5078125" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="67.5" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="52.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -584,20 +587,22 @@
       <c r="W1" s="9" t="s">
         <v>22</v>
       </c>
-      <c r="X1" s="10"/>
+      <c r="X1" s="10" t="s">
+        <v>23</v>
+      </c>
       <c r="Y1" s="10" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B2" s="12" t="n">
         <v>1</v>
       </c>
       <c r="C2" s="12" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="D2" s="12" t="n">
         <v>0</v>
@@ -606,81 +611,81 @@
         <v>1</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B3" s="12" t="n">
         <v>2</v>
       </c>
       <c r="C3" s="12" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="D3" s="12" t="n">
         <v>0</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="F3" s="0" t="n">
         <v>1</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="I3" s="0" t="n">
         <v>0</v>
       </c>
       <c r="J3" s="0" t="s">
+        <v>34</v>
+      </c>
+      <c r="K3" s="0" t="s">
+        <v>35</v>
+      </c>
+      <c r="L3" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="M3" s="0" t="s">
+        <v>37</v>
+      </c>
+      <c r="N3" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="O3" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q3" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="R3" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="S3" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="T3" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="U3" s="0" t="s">
+        <v>40</v>
+      </c>
+      <c r="V3" s="0" t="s">
         <v>33</v>
-      </c>
-      <c r="K3" s="0" t="s">
-        <v>34</v>
-      </c>
-      <c r="L3" s="0" t="s">
-        <v>35</v>
-      </c>
-      <c r="M3" s="0" t="s">
-        <v>36</v>
-      </c>
-      <c r="N3" s="0" t="s">
-        <v>37</v>
-      </c>
-      <c r="O3" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q3" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="R3" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="S3" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="T3" s="0" t="s">
-        <v>38</v>
-      </c>
-      <c r="U3" s="0" t="s">
-        <v>39</v>
-      </c>
-      <c r="V3" s="0" t="s">
-        <v>32</v>
       </c>
       <c r="W3" s="0" t="n">
         <v>1</v>
@@ -694,70 +699,70 @@
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" s="12" t="n">
         <v>3</v>
       </c>
       <c r="C4" s="12" t="s">
-        <v>40</v>
+        <v>41</v>
       </c>
       <c r="D4" s="12" t="n">
         <v>0</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>41</v>
+        <v>42</v>
       </c>
       <c r="F4" s="0" t="n">
         <v>2</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>43</v>
+        <v>44</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>46</v>
+        <v>47</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>50</v>
+        <v>51</v>
       </c>
       <c r="U4" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="V4" s="0" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="W4" s="0" t="n">
         <v>5</v>
       </c>
       <c r="X4" s="0" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
       <c r="Y4" s="13" t="n">
         <v>44561</v>
@@ -765,13 +770,13 @@
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B5" s="12" t="n">
         <v>4</v>
       </c>
       <c r="C5" s="12" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="D5" s="12" t="n">
         <v>0</v>
@@ -780,45 +785,45 @@
         <v>2</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>55</v>
+        <v>56</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="U5" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="V5" s="0" t="s">
-        <v>56</v>
+        <v>57</v>
       </c>
       <c r="W5" s="0" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="X5" s="0" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B6" s="12" t="n">
         <v>5</v>
       </c>
       <c r="C6" s="12" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="D6" s="12" t="n">
         <v>0</v>
@@ -827,42 +832,42 @@
         <v>2</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>42</v>
+        <v>43</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>61</v>
+        <v>62</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="V6" s="0" t="s">
-        <v>62</v>
+        <v>63</v>
       </c>
       <c r="W6" s="0" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="X6" s="0" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="11" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B7" s="12" t="n">
         <v>6</v>
       </c>
       <c r="C7" s="12" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="D7" s="12" t="n">
         <v>0</v>
@@ -871,45 +876,45 @@
         <v>2</v>
       </c>
       <c r="G7" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="I7" s="0" t="s">
+        <v>66</v>
+      </c>
+      <c r="L7" s="0" t="s">
+        <v>67</v>
+      </c>
+      <c r="M7" s="0" t="s">
+        <v>29</v>
+      </c>
+      <c r="N7" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="Q7" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="V7" s="0" t="s">
+        <v>68</v>
+      </c>
+      <c r="W7" s="0" t="s">
         <v>42</v>
-      </c>
-      <c r="I7" s="0" t="s">
-        <v>65</v>
-      </c>
-      <c r="L7" s="0" t="s">
-        <v>66</v>
-      </c>
-      <c r="M7" s="0" t="s">
-        <v>28</v>
-      </c>
-      <c r="N7" s="0" t="s">
-        <v>29</v>
-      </c>
-      <c r="Q7" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="V7" s="0" t="s">
-        <v>67</v>
-      </c>
-      <c r="W7" s="0" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="L8" s="0" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="M8" s="0" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="N8" s="0" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="Q8" s="0" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="V8" s="0" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
     </row>
   </sheetData>

</xml_diff>